<commit_message>
Digital Objects from sheet test
</commit_message>
<xml_diff>
--- a/backend/spec/fixtures/bulk_updater/test_sheet.xlsx
+++ b/backend/spec/fixtures/bulk_updater/test_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laneymcglohon/Desktop/ArchivesSpaceStuff/fork/archivesspace/backend/spec/fixtures/bulk_updater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFB5EE9-DE65-3C4F-8F9B-20C242FB8FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644E1B31-890F-084F-B5C7-B72AF2D0C50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="29000" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="1183">
   <si>
     <t>Id</t>
   </si>
@@ -3558,6 +3558,18 @@
   </si>
   <si>
     <t xml:space="preserve">Lang material note content																																																																																																																																																</t>
+  </si>
+  <si>
+    <t>DOI1</t>
+  </si>
+  <si>
+    <t>DO Title</t>
+  </si>
+  <si>
+    <t>File Caption</t>
+  </si>
+  <si>
+    <t>/dig_obj/file.jpg</t>
   </si>
 </sst>
 </file>
@@ -3925,10 +3937,10 @@
   <dimension ref="A1:GD31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="CS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD31"/>
+      <selection pane="bottomRight" activeCell="DF3" sqref="DF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5173,6 +5185,24 @@
       </c>
       <c r="BO3" s="4" t="s">
         <v>390</v>
+      </c>
+      <c r="DC3" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="DD3" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="DE3" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="DF3" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="DG3" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="DH3" s="4" t="s">
+        <v>421</v>
       </c>
       <c r="EI3" s="4" t="s">
         <v>391</v>
@@ -5951,13 +5981,13 @@
           <x14:formula1>
             <xm:f>Enums!$DE$2:$DE$3</xm:f>
           </x14:formula1>
-          <xm:sqref>DE3:DE32</xm:sqref>
+          <xm:sqref>DE4:DE32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002B000000}">
           <x14:formula1>
             <xm:f>Enums!$DH$2:$DH$3</xm:f>
           </x14:formula1>
-          <xm:sqref>DH3:DH32</xm:sqref>
+          <xm:sqref>DH4:DH32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002C000000}">
           <x14:formula1>

</xml_diff>